<commit_message>
update custom pcb and documentation
#23
</commit_message>
<xml_diff>
--- a/CustomPCB/PowerPCBV2/bom.xlsx
+++ b/CustomPCB/PowerPCBV2/bom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hogeschoolpxl-my.sharepoint.com/personal/11901129_student_pxl_be/Documents/EAI_3de_jaar/stage/RescueDrone/CustomPCB/PowerPCBV2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="147" documentId="8_{11D7C852-2A06-403E-B623-DEC880C1AD1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{15C1C83E-A2D2-41A5-9B72-ED31AA755B21}"/>
+  <xr:revisionPtr revIDLastSave="165" documentId="8_{11D7C852-2A06-403E-B623-DEC880C1AD1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5BF34D2B-4810-4F2D-A27D-FBE6FC3A6937}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="12852" windowWidth="23256" windowHeight="12456" xr2:uid="{426CB744-3008-4D28-AAB0-E99B5ABD92DA}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Blad1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="ExterneGegevens_1" localSheetId="0" hidden="1">PowerPCBV2!$A$1:$H$20</definedName>
+    <definedName name="ExterneGegevens_1" localSheetId="0" hidden="1">PowerPCBV2!$A$1:$H$21</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="55">
   <si>
     <t/>
   </si>
@@ -145,60 +145,15 @@
     <t>Collated Components:</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>CB1, CB2</t>
   </si>
   <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
     <t>D1, D2</t>
   </si>
   <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
     <t>Sin1, Sout1</t>
   </si>
   <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
     <t>Component Count:</t>
   </si>
   <si>
@@ -248,6 +203,15 @@
   </si>
   <si>
     <t>Qty one PCB</t>
+  </si>
+  <si>
+    <t>Cin-HF1, Cin-HF2, Cout-HF1, Cout-HF2</t>
+  </si>
+  <si>
+    <t>0,47uF</t>
+  </si>
+  <si>
+    <t>470nF cap</t>
   </si>
 </sst>
 </file>
@@ -292,11 +256,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -368,8 +335,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C9344FB7-3EB5-4534-A8BB-C6F77D974F5D}" name="PowerPCBV2" displayName="PowerPCBV2" ref="A1:H20" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:H20" xr:uid="{C9344FB7-3EB5-4534-A8BB-C6F77D974F5D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C9344FB7-3EB5-4534-A8BB-C6F77D974F5D}" name="PowerPCBV2" displayName="PowerPCBV2" ref="A1:H21" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:H21" xr:uid="{C9344FB7-3EB5-4534-A8BB-C6F77D974F5D}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{51BEA293-38C4-407B-988B-19F4BC64C295}" uniqueName="1" name="Item" queryTableFieldId="1" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{AB4EF3BD-398A-4145-A91E-0718841B0758}" uniqueName="2" name="Qty one PCB" queryTableFieldId="2" dataDxfId="6"/>
@@ -683,17 +650,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4356865-E6D2-449C-AEB2-79A9DACB70FB}">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.42578125" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
@@ -706,25 +673,25 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="G1" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="H1" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -750,20 +717,20 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>32</v>
+      <c r="A3" s="1">
+        <v>1</v>
       </c>
       <c r="B3" s="3">
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="F3" s="1">
         <v>3</v>
@@ -773,407 +740,427 @@
         <v>6</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="1">
+        <f>A3+1</f>
+        <v>2</v>
+      </c>
+      <c r="B4" s="4">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" s="1">
+        <v>3</v>
+      </c>
+      <c r="G4" s="1">
+        <f>PowerPCBV2[[#This Row],[Qty one PCB]]*PowerPCBV2[[#This Row],[multiple]]</f>
+        <v>12</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <f t="shared" ref="A5:A18" si="0">A4+1</f>
+        <v>3</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="1">
+        <v>3</v>
+      </c>
+      <c r="G5" s="1">
+        <f>PowerPCBV2[[#This Row],[Qty one PCB]]*PowerPCBV2[[#This Row],[multiple]]</f>
+        <v>3</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B6" s="3">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" s="1">
+        <v>3</v>
+      </c>
+      <c r="G6" s="1">
+        <f>PowerPCBV2[[#This Row],[Qty one PCB]]*PowerPCBV2[[#This Row],[multiple]]</f>
+        <v>3</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B7" s="3">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="1">
+        <v>3</v>
+      </c>
+      <c r="G7" s="1">
+        <f>PowerPCBV2[[#This Row],[Qty one PCB]]*PowerPCBV2[[#This Row],[multiple]]</f>
+        <v>3</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B8" s="3">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="1">
+        <v>3</v>
+      </c>
+      <c r="G8" s="1">
+        <f>PowerPCBV2[[#This Row],[Qty one PCB]]*PowerPCBV2[[#This Row],[multiple]]</f>
+        <v>3</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B9" s="3">
+        <v>2</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="3">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="D9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="1">
+        <v>3</v>
+      </c>
+      <c r="G9" s="1">
+        <f>PowerPCBV2[[#This Row],[Qty one PCB]]*PowerPCBV2[[#This Row],[multiple]]</f>
         <v>6</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="F4" s="1">
-        <v>3</v>
-      </c>
-      <c r="G4" s="1">
-        <f>PowerPCBV2[[#This Row],[Qty one PCB]]*PowerPCBV2[[#This Row],[multiple]]</f>
-        <v>3</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="3">
-        <v>1</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="1" t="s">
+      <c r="H9" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F5" s="1">
-        <v>3</v>
-      </c>
-      <c r="G5" s="1">
-        <f>PowerPCBV2[[#This Row],[Qty one PCB]]*PowerPCBV2[[#This Row],[multiple]]</f>
-        <v>3</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="3">
-        <v>1</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="B10" s="3">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1">
+        <f>PowerPCBV2[[#This Row],[Qty one PCB]]*PowerPCBV2[[#This Row],[multiple]]</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="B11" s="3">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1">
+        <f>PowerPCBV2[[#This Row],[Qty one PCB]]*PowerPCBV2[[#This Row],[multiple]]</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="F6" s="1">
-        <v>3</v>
-      </c>
-      <c r="G6" s="1">
-        <f>PowerPCBV2[[#This Row],[Qty one PCB]]*PowerPCBV2[[#This Row],[multiple]]</f>
-        <v>3</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" s="3">
-        <v>1</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="B12" s="3">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1">
+        <f>PowerPCBV2[[#This Row],[Qty one PCB]]*PowerPCBV2[[#This Row],[multiple]]</f>
+        <v>0</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="B13" s="3">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0</v>
+      </c>
+      <c r="G13" s="1">
+        <f>PowerPCBV2[[#This Row],[Qty one PCB]]*PowerPCBV2[[#This Row],[multiple]]</f>
+        <v>0</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="F7" s="1">
-        <v>3</v>
-      </c>
-      <c r="G7" s="1">
-        <f>PowerPCBV2[[#This Row],[Qty one PCB]]*PowerPCBV2[[#This Row],[multiple]]</f>
-        <v>3</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" s="3">
+      <c r="B14" s="3">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" s="1">
+        <v>3</v>
+      </c>
+      <c r="G14" s="1">
+        <f>PowerPCBV2[[#This Row],[Qty one PCB]]*PowerPCBV2[[#This Row],[multiple]]</f>
+        <v>3</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B15" s="3">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="1">
+        <v>3</v>
+      </c>
+      <c r="G15" s="1">
+        <f>PowerPCBV2[[#This Row],[Qty one PCB]]*PowerPCBV2[[#This Row],[multiple]]</f>
+        <v>3</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B16" s="3">
         <v>2</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0</v>
+      </c>
+      <c r="G16" s="1">
+        <f>PowerPCBV2[[#This Row],[Qty one PCB]]*PowerPCBV2[[#This Row],[multiple]]</f>
+        <v>0</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B17" s="3">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F8" s="1">
-        <v>3</v>
-      </c>
-      <c r="G8" s="1">
-        <f>PowerPCBV2[[#This Row],[Qty one PCB]]*PowerPCBV2[[#This Row],[multiple]]</f>
-        <v>6</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B9" s="3">
-        <v>1</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="1">
-        <v>0</v>
-      </c>
-      <c r="G9" s="1">
-        <f>PowerPCBV2[[#This Row],[Qty one PCB]]*PowerPCBV2[[#This Row],[multiple]]</f>
-        <v>0</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B10" s="3">
-        <v>1</v>
-      </c>
-      <c r="C10" s="1" t="s">
+      <c r="F17" s="1">
+        <v>3</v>
+      </c>
+      <c r="G17" s="1">
+        <f>PowerPCBV2[[#This Row],[Qty one PCB]]*PowerPCBV2[[#This Row],[multiple]]</f>
+        <v>3</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="1">
-        <v>0</v>
-      </c>
-      <c r="G10" s="1">
-        <f>PowerPCBV2[[#This Row],[Qty one PCB]]*PowerPCBV2[[#This Row],[multiple]]</f>
-        <v>0</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B11" s="3">
-        <v>1</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F11" s="1">
-        <v>0</v>
-      </c>
-      <c r="G11" s="1">
-        <f>PowerPCBV2[[#This Row],[Qty one PCB]]*PowerPCBV2[[#This Row],[multiple]]</f>
-        <v>0</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B12" s="3">
-        <v>1</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F12" s="1">
-        <v>0</v>
-      </c>
-      <c r="G12" s="1">
-        <f>PowerPCBV2[[#This Row],[Qty one PCB]]*PowerPCBV2[[#This Row],[multiple]]</f>
-        <v>0</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B13" s="3">
-        <v>1</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F13" s="1">
-        <v>3</v>
-      </c>
-      <c r="G13" s="1">
-        <f>PowerPCBV2[[#This Row],[Qty one PCB]]*PowerPCBV2[[#This Row],[multiple]]</f>
-        <v>3</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B14" s="3">
-        <v>1</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F14" s="1">
-        <v>3</v>
-      </c>
-      <c r="G14" s="1">
-        <f>PowerPCBV2[[#This Row],[Qty one PCB]]*PowerPCBV2[[#This Row],[multiple]]</f>
-        <v>3</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B15" s="3">
-        <v>2</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F15" s="1">
-        <v>0</v>
-      </c>
-      <c r="G15" s="1">
-        <f>PowerPCBV2[[#This Row],[Qty one PCB]]*PowerPCBV2[[#This Row],[multiple]]</f>
-        <v>0</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B16" s="3">
-        <v>1</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F16" s="1">
-        <v>3</v>
-      </c>
-      <c r="G16" s="1">
-        <f>PowerPCBV2[[#This Row],[Qty one PCB]]*PowerPCBV2[[#This Row],[multiple]]</f>
-        <v>3</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B17" s="3">
-        <v>1</v>
-      </c>
-      <c r="C17" s="1" t="s">
+      <c r="B18" s="3">
+        <v>1</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F17" s="1">
-        <v>3</v>
-      </c>
-      <c r="G17" s="1">
-        <f>PowerPCBV2[[#This Row],[Qty one PCB]]*PowerPCBV2[[#This Row],[multiple]]</f>
-        <v>3</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1" t="s">
-        <v>0</v>
+      <c r="E18" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F18" s="1">
+        <v>3</v>
+      </c>
+      <c r="G18" s="1">
+        <f>PowerPCBV2[[#This Row],[Qty one PCB]]*PowerPCBV2[[#This Row],[multiple]]</f>
+        <v>3</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1200,11 +1187,10 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B20" s="1">
-        <f>SUBTOTAL(109,B2:B19)</f>
-        <v>18</v>
+        <v>0</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>0</v>
@@ -1216,49 +1202,74 @@
         <v>0</v>
       </c>
       <c r="F20" s="1"/>
-      <c r="G20" s="1">
-        <f>SUBTOTAL(109,G2:G19)</f>
-        <v>36</v>
-      </c>
+      <c r="G20" s="1"/>
       <c r="H20" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="1">
+        <f>SUBTOTAL(109,B2:B20)</f>
+        <v>22</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1">
+        <f>SUBTOTAL(109,G2:G20)</f>
+        <v>48</v>
+      </c>
+      <c r="H21" s="1" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H8" r:id="rId1" xr:uid="{00CE4474-0971-44EE-B35A-C68D4F158413}"/>
-    <hyperlink ref="E16" r:id="rId2" xr:uid="{9CEA3217-70F4-4D73-AF9D-E9DEAA10F5C6}"/>
-    <hyperlink ref="E17" r:id="rId3" xr:uid="{567058DB-214A-492B-B775-2C50FC349275}"/>
-    <hyperlink ref="H16" r:id="rId4" xr:uid="{9E01766E-CE20-4E20-8C6E-2EC570015DD9}"/>
-    <hyperlink ref="H17" r:id="rId5" xr:uid="{EBA68756-A516-4CFE-BEAB-E85379AB94FD}"/>
-    <hyperlink ref="H13" r:id="rId6" xr:uid="{5A8E7B05-872D-4752-AE10-6A53618F9333}"/>
-    <hyperlink ref="H14" r:id="rId7" xr:uid="{139520F3-1B03-4372-8C20-6DE7768465D4}"/>
-    <hyperlink ref="E4" r:id="rId8" xr:uid="{08C91947-E03B-4302-BF09-919F27E6CA1E}"/>
-    <hyperlink ref="E8" r:id="rId9" xr:uid="{A366A48E-2301-4441-A56F-D313388890AB}"/>
-    <hyperlink ref="E6" r:id="rId10" xr:uid="{5DF74681-BF25-4B9E-8DC3-D67B5C2E691F}"/>
-    <hyperlink ref="E7" r:id="rId11" xr:uid="{A17BF167-9A90-4DE8-A6CF-8E67F4C750BE}"/>
-    <hyperlink ref="H6" r:id="rId12" xr:uid="{21D1F560-F7C1-494C-85F1-9380125BA8B2}"/>
-    <hyperlink ref="H4" r:id="rId13" xr:uid="{53E36744-8F1C-4D97-9519-EEDBE4A84FE6}"/>
-    <hyperlink ref="H7" r:id="rId14" xr:uid="{9E8B1C6B-60AF-43CA-889A-301547A0342F}"/>
-    <hyperlink ref="H5" r:id="rId15" xr:uid="{AB8765F9-FFA4-4F74-86D4-8EE380D4EC1A}"/>
-    <hyperlink ref="E5" r:id="rId16" xr:uid="{C6B5857A-2446-42B7-B8D8-E460A15E621D}"/>
+    <hyperlink ref="H9" r:id="rId1" xr:uid="{00CE4474-0971-44EE-B35A-C68D4F158413}"/>
+    <hyperlink ref="E17" r:id="rId2" xr:uid="{9CEA3217-70F4-4D73-AF9D-E9DEAA10F5C6}"/>
+    <hyperlink ref="E18" r:id="rId3" xr:uid="{567058DB-214A-492B-B775-2C50FC349275}"/>
+    <hyperlink ref="H17" r:id="rId4" xr:uid="{9E01766E-CE20-4E20-8C6E-2EC570015DD9}"/>
+    <hyperlink ref="H18" r:id="rId5" xr:uid="{EBA68756-A516-4CFE-BEAB-E85379AB94FD}"/>
+    <hyperlink ref="H14" r:id="rId6" xr:uid="{5A8E7B05-872D-4752-AE10-6A53618F9333}"/>
+    <hyperlink ref="H15" r:id="rId7" xr:uid="{139520F3-1B03-4372-8C20-6DE7768465D4}"/>
+    <hyperlink ref="E5" r:id="rId8" xr:uid="{08C91947-E03B-4302-BF09-919F27E6CA1E}"/>
+    <hyperlink ref="E9" r:id="rId9" xr:uid="{A366A48E-2301-4441-A56F-D313388890AB}"/>
+    <hyperlink ref="E7" r:id="rId10" xr:uid="{5DF74681-BF25-4B9E-8DC3-D67B5C2E691F}"/>
+    <hyperlink ref="E8" r:id="rId11" xr:uid="{A17BF167-9A90-4DE8-A6CF-8E67F4C750BE}"/>
+    <hyperlink ref="H7" r:id="rId12" xr:uid="{21D1F560-F7C1-494C-85F1-9380125BA8B2}"/>
+    <hyperlink ref="H5" r:id="rId13" xr:uid="{53E36744-8F1C-4D97-9519-EEDBE4A84FE6}"/>
+    <hyperlink ref="H8" r:id="rId14" xr:uid="{9E8B1C6B-60AF-43CA-889A-301547A0342F}"/>
+    <hyperlink ref="H6" r:id="rId15" xr:uid="{AB8765F9-FFA4-4F74-86D4-8EE380D4EC1A}"/>
+    <hyperlink ref="E6" r:id="rId16" xr:uid="{C6B5857A-2446-42B7-B8D8-E460A15E621D}"/>
     <hyperlink ref="H3" r:id="rId17" xr:uid="{5D42272B-24E3-49D5-8597-25DB5E40261C}"/>
     <hyperlink ref="E3" r:id="rId18" xr:uid="{98E62FB8-2E69-452F-91E7-23CE8B7540CD}"/>
-    <hyperlink ref="E9" r:id="rId19" xr:uid="{8F2D9D73-722A-4CA5-8300-4B48839100F2}"/>
-    <hyperlink ref="E10" r:id="rId20" xr:uid="{5174D3CF-3FD5-4601-8906-B9149C7EC02A}"/>
-    <hyperlink ref="E11" r:id="rId21" xr:uid="{F290E2BA-F893-441A-B6CF-5E77684AA574}"/>
-    <hyperlink ref="E12" r:id="rId22" xr:uid="{80D4B1A9-2DDC-492E-8B05-F30A14E9258E}"/>
-    <hyperlink ref="H15" r:id="rId23" xr:uid="{11E85DA5-B9BF-4910-8245-B63ABA025AC4}"/>
-    <hyperlink ref="H9" r:id="rId24" xr:uid="{AAA84C4C-C13F-4A29-9986-5F8E0C457040}"/>
-    <hyperlink ref="H10" r:id="rId25" xr:uid="{97993F24-7B8F-41F0-B4C6-0470D645EFF6}"/>
-    <hyperlink ref="H11" r:id="rId26" xr:uid="{4FE385E6-C795-48FA-8A34-865845839E2B}"/>
-    <hyperlink ref="H12" r:id="rId27" xr:uid="{B898EA3E-29F7-4B95-8201-29EFE7F2576D}"/>
-    <hyperlink ref="E13" r:id="rId28" xr:uid="{81BCBBB8-AB5E-48DF-B336-A660687D7010}"/>
-    <hyperlink ref="E14" r:id="rId29" xr:uid="{53A30FF4-102C-481F-A2BB-7F7A2ADD4D56}"/>
+    <hyperlink ref="E10" r:id="rId19" xr:uid="{8F2D9D73-722A-4CA5-8300-4B48839100F2}"/>
+    <hyperlink ref="E11" r:id="rId20" xr:uid="{5174D3CF-3FD5-4601-8906-B9149C7EC02A}"/>
+    <hyperlink ref="E12" r:id="rId21" xr:uid="{F290E2BA-F893-441A-B6CF-5E77684AA574}"/>
+    <hyperlink ref="E13" r:id="rId22" xr:uid="{80D4B1A9-2DDC-492E-8B05-F30A14E9258E}"/>
+    <hyperlink ref="H16" r:id="rId23" xr:uid="{11E85DA5-B9BF-4910-8245-B63ABA025AC4}"/>
+    <hyperlink ref="H10" r:id="rId24" xr:uid="{AAA84C4C-C13F-4A29-9986-5F8E0C457040}"/>
+    <hyperlink ref="H11" r:id="rId25" xr:uid="{97993F24-7B8F-41F0-B4C6-0470D645EFF6}"/>
+    <hyperlink ref="H12" r:id="rId26" xr:uid="{4FE385E6-C795-48FA-8A34-865845839E2B}"/>
+    <hyperlink ref="H13" r:id="rId27" xr:uid="{B898EA3E-29F7-4B95-8201-29EFE7F2576D}"/>
+    <hyperlink ref="E14" r:id="rId28" xr:uid="{81BCBBB8-AB5E-48DF-B336-A660687D7010}"/>
+    <hyperlink ref="E15" r:id="rId29" xr:uid="{53A30FF4-102C-481F-A2BB-7F7A2ADD4D56}"/>
+    <hyperlink ref="E4" r:id="rId30" xr:uid="{203A6400-09C1-4A1A-A7E3-DB507009F96F}"/>
+    <hyperlink ref="H4" r:id="rId31" xr:uid="{A6DC1F51-A42D-4CC9-8545-CB439F7A564B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId30"/>
+    <tablePart r:id="rId32"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>